<commit_message>
Ändrade funktionen clean data
</commit_message>
<xml_diff>
--- a/basmetadata_extern_webb.xlsx
+++ b/basmetadata_extern_webb.xlsx
@@ -45,61 +45,61 @@
     <t xml:space="preserve">Serie </t>
   </si>
   <si>
-    <t>Klassificeringsstruktur</t>
-  </si>
-  <si>
     <t>Ursprung</t>
   </si>
   <si>
+    <t>Personuppgifter</t>
+  </si>
+  <si>
+    <t>Forskningsdata</t>
+  </si>
+  <si>
+    <t>Kommentar</t>
+  </si>
+  <si>
+    <t>Arkivering av webbsidor</t>
+  </si>
+  <si>
+    <t>Gislaveds kommun</t>
+  </si>
+  <si>
+    <t>nivå2</t>
+  </si>
+  <si>
+    <t>nivå3</t>
+  </si>
+  <si>
+    <t>Basmetadata</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Webbpubliceringsverktyget Sitevision</t>
+  </si>
+  <si>
+    <t>Gislaveds Externa webb</t>
+  </si>
+  <si>
+    <t>3.4.1 Extern webb</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>KlassificeringsstrukturText</t>
+  </si>
+  <si>
     <t>Sekretess</t>
   </si>
   <si>
-    <t>Personuppgifter</t>
-  </si>
-  <si>
-    <t>Forskningsdata</t>
-  </si>
-  <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Arkivering av webbsidor</t>
-  </si>
-  <si>
-    <t>Gislaveds kommun</t>
-  </si>
-  <si>
     <t>nivå1</t>
-  </si>
-  <si>
-    <t>nivå2</t>
-  </si>
-  <si>
-    <t>nivå3</t>
-  </si>
-  <si>
-    <t>Basmetadata</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Webbpubliceringsverktyget Sitevision</t>
-  </si>
-  <si>
-    <t>Gislaveds Externa webb</t>
-  </si>
-  <si>
-    <t>3.4.1 Extern webb</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -421,7 +421,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -432,10 +432,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -475,52 +475,52 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -544,10 +544,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>